<commit_message>
Finish UT Stats Course, Part 1
</commit_message>
<xml_diff>
--- a/Stats/UT/UT.7.11xFoundationsofData Analysis.1/wk6.xlsx
+++ b/Stats/UT/UT.7.11xFoundationsofData Analysis.1/wk6.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>The spread of this season's flu virus can be modeled logistically.  A group of 500 people were initially infected in a town of 75,000 people.  One month later, 750 people were infected.</t>
   </si>
@@ -93,13 +93,43 @@
   </si>
   <si>
     <t>pop after 5 yrs</t>
+  </si>
+  <si>
+    <t>= b</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Flu Cases</t>
+  </si>
+  <si>
+    <t>Rate of Change</t>
+  </si>
+  <si>
+    <t>Rate of Change %</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Years since Project Began</t>
+  </si>
+  <si>
+    <t>Number of Wolves</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,16 +145,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,16 +181,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC8C8C8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC8C8C8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC8C8C8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC8C8C8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +685,9 @@
         <f>1/D13</f>
         <v>1.505050505050505</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -625,6 +701,319 @@
       </c>
       <c r="E14" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>73</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1996</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>42853</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>105</v>
+      </c>
+      <c r="D20">
+        <f>C20-C19</f>
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <f>(C20/C19)-1</f>
+        <v>0.43835616438356162</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1998</v>
+      </c>
+      <c r="I20" s="7">
+        <v>3</v>
+      </c>
+      <c r="J20" s="7">
+        <v>45</v>
+      </c>
+      <c r="K20">
+        <f>J20-J19</f>
+        <v>20</v>
+      </c>
+      <c r="L20">
+        <f>(J20/J19)-1</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>42854</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>137</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D28" si="0">C21-C20</f>
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E28" si="1">(C21/C20)-1</f>
+        <v>0.30476190476190479</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21" si="2">J21-J20</f>
+        <v>-45</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21" si="3">(J21/J20)-1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>42855</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>257</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.87591240875912413</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42856</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>367</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.42801556420233466</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>658</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>291</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.79291553133514991</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42858</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>898</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0.36474164133738607</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>42859</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1085</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0.2082405345211582</v>
+      </c>
+      <c r="H26">
+        <v>1995</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>42860</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1490</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>405</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.37327188940092171</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1996</v>
+      </c>
+      <c r="I27" s="7">
+        <v>1</v>
+      </c>
+      <c r="J27" s="7">
+        <v>25</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:K29" si="4">J27-J26</f>
+        <v>10</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" ref="L27:L29" si="5">(J27/J26)-1</f>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>42861</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1893</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0.27046979865771803</v>
+      </c>
+      <c r="H28" s="7">
+        <v>1997</v>
+      </c>
+      <c r="I28" s="7">
+        <v>2</v>
+      </c>
+      <c r="J28" s="7">
+        <v>35</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="5"/>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H29" s="7">
+        <v>1998</v>
+      </c>
+      <c r="I29" s="7">
+        <v>3</v>
+      </c>
+      <c r="J29" s="7">
+        <v>45</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="L29" s="9">
+        <f t="shared" si="5"/>
+        <v>0.28571428571428581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>